<commit_message>
gestion auto liste comp
</commit_message>
<xml_diff>
--- a/src/main/resources/template/formations_template.xlsx
+++ b/src/main/resources/template/formations_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Libelle</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>${form.infoCompFormStr}</t>
+  </si>
+  <si>
+    <t>Date confirm. Liste comp.</t>
+  </si>
+  <si>
+    <t>${form.datConfirmListCompFormStr}</t>
   </si>
 </sst>
 </file>
@@ -587,12 +593,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="Z3" sqref="Z3"/>
+      <selection pane="bottomLeft" activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -618,17 +624,18 @@
     <col min="20" max="20" width="17.5703125" style="4" customWidth="1"/>
     <col min="21" max="21" width="19.85546875" style="4" customWidth="1"/>
     <col min="22" max="22" width="21.42578125" style="4" customWidth="1"/>
-    <col min="23" max="23" width="23.5703125" style="4" customWidth="1"/>
-    <col min="24" max="24" width="22.42578125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="23.5703125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="31.85546875" style="4" customWidth="1"/>
-    <col min="27" max="27" width="24.5703125" style="4" customWidth="1"/>
-    <col min="28" max="28" width="17.7109375" style="4" customWidth="1"/>
-    <col min="29" max="29" width="25.140625" style="4" customWidth="1"/>
-    <col min="30" max="30" width="26.140625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="27" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.5703125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="22.42578125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="23.5703125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="31.85546875" style="4" customWidth="1"/>
+    <col min="28" max="28" width="24.5703125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.7109375" style="4" customWidth="1"/>
+    <col min="30" max="30" width="25.140625" style="4" customWidth="1"/>
+    <col min="31" max="31" width="26.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -696,31 +703,34 @@
         <v>10</v>
       </c>
       <c r="W1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -788,31 +798,34 @@
         <v>47</v>
       </c>
       <c r="W2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -838,11 +851,12 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="6"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>